<commit_message>
update scenarios one last time for pub
</commit_message>
<xml_diff>
--- a/data/scenarios.xlsx
+++ b/data/scenarios.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://iiasahub-my.sharepoint.com/personal/gidden_iiasa_ac_at/Documents/work/iiasa/papers/dac-fairness-feasibility/gidden_brutschin_et_al_2023/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="817" documentId="11_AB6950C68BE577815F655C903F0D020999345216" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7070AB48-F738-418C-ADB3-83BF83AB6124}"/>
+  <xr:revisionPtr revIDLastSave="896" documentId="11_AB6950C68BE577815F655C903F0D020999345216" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76EA75E8-538A-4230-B508-A316746925AB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="core" sheetId="9" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="governance" sheetId="11" r:id="rId3"/>
     <sheet name="equity_comparison" sheetId="13" r:id="rId4"/>
     <sheet name="scenario_table" sheetId="14" r:id="rId5"/>
+    <sheet name="assumption table" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="658" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -253,13 +254,61 @@
   </si>
   <si>
     <t>Core</t>
+  </si>
+  <si>
+    <t>Climate</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Cumulative Carbon Budget</t>
+  </si>
+  <si>
+    <t>500 Gt</t>
+  </si>
+  <si>
+    <t>1.5C-OS</t>
+  </si>
+  <si>
+    <t>700 Gt</t>
+  </si>
+  <si>
+    <t>1000 Gt</t>
+  </si>
+  <si>
+    <t>DACCS Maximum Diffusion</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>10% + 5%*</t>
+  </si>
+  <si>
+    <t>DACCS Technoeconomic Assumptions</t>
+  </si>
+  <si>
+    <t>See SI Table 2</t>
+  </si>
+  <si>
+    <t>Governance Assumptions</t>
+  </si>
+  <si>
+    <t>SSP Scenario</t>
+  </si>
+  <si>
+    <t>See SI Table 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +322,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,6 +352,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -559,6 +633,54 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1991,7 +2113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FADE4FE-2402-42D1-ABBB-07D12D880BB0}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2262,10 +2384,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC1781E-ED30-4178-91D0-BEC0AAC3190C}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2273,14 +2395,14 @@
     <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="62.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="44" t="s">
         <v>70</v>
       </c>
@@ -2291,25 +2413,22 @@
         <v>4</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="37" t="s">
         <v>6</v>
       </c>
+      <c r="E1" s="38" t="s">
+        <v>7</v>
+      </c>
       <c r="F1" s="38" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G1" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="H1" s="39" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
         <v>71</v>
       </c>
@@ -2320,25 +2439,22 @@
         <v>15</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G2" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="30" t="s">
         <v>71</v>
       </c>
@@ -2349,25 +2465,22 @@
         <v>23</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>71</v>
       </c>
@@ -2378,25 +2491,22 @@
         <v>26</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G4" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
         <v>71</v>
       </c>
@@ -2407,7 +2517,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>29</v>
@@ -2416,16 +2526,13 @@
         <v>29</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>71</v>
       </c>
@@ -2436,7 +2543,7 @@
         <v>23</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>29</v>
@@ -2445,16 +2552,13 @@
         <v>29</v>
       </c>
       <c r="G6" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H6" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>71</v>
       </c>
@@ -2465,7 +2569,7 @@
         <v>26</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="E7" s="25" t="s">
         <v>29</v>
@@ -2474,16 +2578,13 @@
         <v>29</v>
       </c>
       <c r="G7" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>8</v>
       </c>
@@ -2494,25 +2595,22 @@
         <v>15</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F8" s="26" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G8" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>8</v>
       </c>
@@ -2523,25 +2621,22 @@
         <v>23</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F9" s="31" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="30" t="s">
         <v>8</v>
       </c>
@@ -2552,25 +2647,22 @@
         <v>15</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F10" s="31" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G10" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
         <v>8</v>
       </c>
@@ -2581,25 +2673,22 @@
         <v>23</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F11" s="31" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H11" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>8</v>
       </c>
@@ -2610,25 +2699,22 @@
         <v>15</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G12" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="30" t="s">
         <v>8</v>
       </c>
@@ -2639,25 +2725,22 @@
         <v>23</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I13" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="30" t="s">
         <v>8</v>
       </c>
@@ -2668,25 +2751,22 @@
         <v>15</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14" s="31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G14" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="30" t="s">
         <v>8</v>
       </c>
@@ -2697,25 +2777,22 @@
         <v>23</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F15" s="31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H15" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
         <v>8</v>
       </c>
@@ -2726,25 +2803,22 @@
         <v>26</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F16" s="31" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="G16" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I16" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
         <v>8</v>
       </c>
@@ -2755,25 +2829,22 @@
         <v>26</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="F17" s="31" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H17" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
         <v>8</v>
       </c>
@@ -2784,25 +2855,22 @@
         <v>26</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G18" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H18" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30" t="s">
         <v>8</v>
       </c>
@@ -2813,25 +2881,22 @@
         <v>26</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="25" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G19" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="H19" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="I19" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H19" s="32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
         <v>9</v>
       </c>
@@ -2842,25 +2907,22 @@
         <v>15</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" s="26" t="s">
         <v>18</v>
       </c>
       <c r="G20" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="H20" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="I20" s="29" t="s">
+      <c r="H20" s="29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="30" t="s">
         <v>9</v>
       </c>
@@ -2871,25 +2933,22 @@
         <v>15</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" s="31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H21" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I21" s="32" t="s">
+      <c r="H21" s="32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="30" t="s">
         <v>9</v>
       </c>
@@ -2900,25 +2959,22 @@
         <v>15</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F22" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G22" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I22" s="32" t="s">
+      <c r="H22" s="32" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="30" t="s">
         <v>9</v>
       </c>
@@ -2929,25 +2985,22 @@
         <v>15</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H23" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="32" t="s">
+      <c r="H23" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="30" t="s">
         <v>9</v>
       </c>
@@ -2958,25 +3011,22 @@
         <v>15</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G24" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H24" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I24" s="32" t="s">
+      <c r="H24" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="30" t="s">
         <v>9</v>
       </c>
@@ -2987,25 +3037,22 @@
         <v>15</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I25" s="32" t="s">
+      <c r="H25" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="30" t="s">
         <v>9</v>
       </c>
@@ -3016,25 +3063,22 @@
         <v>26</v>
       </c>
       <c r="D26" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F26" s="31" t="s">
         <v>18</v>
       </c>
       <c r="G26" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="H26" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="32" t="s">
+      <c r="H26" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="30" t="s">
         <v>9</v>
       </c>
@@ -3045,25 +3089,22 @@
         <v>26</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27" s="31" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I27" s="32" t="s">
+      <c r="H27" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="30" t="s">
         <v>9</v>
       </c>
@@ -3074,25 +3115,22 @@
         <v>26</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F28" s="31" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="G28" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="H28" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="I28" s="32" t="s">
+      <c r="H28" s="32" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>9</v>
       </c>
@@ -3103,25 +3141,168 @@
         <v>23</v>
       </c>
       <c r="D29" s="25" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F29" s="25" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="H29" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="I29" s="34" t="s">
+      <c r="H29" s="34" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EB6369-A546-4978-A63B-987665640D1D}">
+  <dimension ref="A1:H5"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="46" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="48"/>
+      <c r="C1" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="48"/>
+      <c r="E1" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="48"/>
+      <c r="G1" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="H1" s="48"/>
+    </row>
+    <row r="2" spans="1:8" s="46" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="49" t="s">
+        <v>80</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="G2" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="57">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="52" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="54" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="58">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="60" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>